<commit_message>
removed fiona code and finalized db_building
</commit_message>
<xml_diff>
--- a/conceptual test/master.xlsx
+++ b/conceptual test/master.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lorenzorinaldi/Documents/GitHub/SESAM/FIONA/conceptual test/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBDE5EA3-2CCF-644B-9733-4CB361C66EF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{410251B2-22A5-984A-82A3-B181A190EB86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17460" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Master" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="41">
   <si>
     <t>Region</t>
   </si>
@@ -144,9 +144,6 @@
   </si>
   <si>
     <t>ACT2</t>
-  </si>
-  <si>
-    <t>COM2</t>
   </si>
   <si>
     <t>new_act2</t>
@@ -565,8 +562,8 @@
   </sheetPr>
   <dimension ref="A1:L3"/>
   <sheetViews>
-    <sheetView zoomScale="179" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3:L3"/>
+    <sheetView tabSelected="1" zoomScale="179" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -657,16 +654,16 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B3" t="s">
         <v>39</v>
       </c>
       <c r="C3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D3" t="s">
         <v>40</v>
-      </c>
-      <c r="D3" t="s">
-        <v>41</v>
       </c>
       <c r="E3" s="3">
         <v>1</v>
@@ -731,7 +728,7 @@
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -792,10 +789,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{134A2002-F26B-0243-A606-48AF09AA929E}">
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="172" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView zoomScale="172" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -846,32 +843,9 @@
         <v>27</v>
       </c>
       <c r="F2" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="G2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A3">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" t="s">
-        <v>38</v>
-      </c>
-      <c r="D3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E3" t="s">
-        <v>38</v>
-      </c>
-      <c r="F3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G3" t="s">
         <v>35</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Issue n.1 solved: new activities can consume new commodities supplied by other new activities
</commit_message>
<xml_diff>
--- a/conceptual test/master.xlsx
+++ b/conceptual test/master.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lorenzorinaldi/Documents/GitHub/SESAM/FIONA/conceptual test/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBDE5EA3-2CCF-644B-9733-4CB361C66EF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA2C695C-0757-FB48-B99D-4AC522853E5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17460" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Master" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="41">
   <si>
     <t>Region</t>
   </si>
@@ -66,9 +66,6 @@
   </si>
   <si>
     <t>unit</t>
-  </si>
-  <si>
-    <t>Final demand</t>
   </si>
   <si>
     <t>test</t>
@@ -565,8 +562,8 @@
   </sheetPr>
   <dimension ref="A1:L3"/>
   <sheetViews>
-    <sheetView zoomScale="179" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3:L3"/>
+    <sheetView tabSelected="1" zoomScale="179" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -625,16 +622,16 @@
     </row>
     <row r="2" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C2" t="s">
         <v>37</v>
       </c>
-      <c r="C2" t="s">
-        <v>38</v>
-      </c>
       <c r="D2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E2" s="3">
         <v>1</v>
@@ -645,14 +642,8 @@
       <c r="G2" s="3">
         <v>1</v>
       </c>
-      <c r="H2">
-        <v>1</v>
-      </c>
-      <c r="I2" t="s">
+      <c r="L2" t="s">
         <v>14</v>
-      </c>
-      <c r="L2" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
@@ -660,31 +651,25 @@
         <v>16</v>
       </c>
       <c r="B3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C3" t="s">
         <v>39</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>40</v>
       </c>
-      <c r="D3" t="s">
-        <v>41</v>
-      </c>
-      <c r="E3" s="3">
+      <c r="E3" s="4">
         <v>1</v>
       </c>
       <c r="F3" t="s">
         <v>13</v>
       </c>
-      <c r="G3" s="3">
-        <v>1</v>
-      </c>
-      <c r="H3">
-        <v>1</v>
-      </c>
-      <c r="I3" t="s">
+      <c r="G3" s="4">
+        <v>1</v>
+      </c>
+      <c r="L3" t="s">
         <v>14</v>
-      </c>
-      <c r="L3" t="s">
-        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -713,12 +698,12 @@
     </row>
     <row r="2" spans="1:1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -730,33 +715,33 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView zoomScale="108" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="C1" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="D1" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="E1" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="F1" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="G1" s="5" t="s">
         <v>23</v>
-      </c>
-      <c r="G1" s="5" t="s">
-        <v>24</v>
       </c>
       <c r="H1" s="5" t="s">
         <v>11</v>
@@ -767,22 +752,22 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D2" t="s">
         <v>2</v>
       </c>
       <c r="E2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F2" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="G2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -792,10 +777,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{134A2002-F26B-0243-A606-48AF09AA929E}">
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="172" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView zoomScale="172" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -805,25 +790,25 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="C1" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="D1" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="E1" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="F1" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="G1" s="5" t="s">
         <v>23</v>
-      </c>
-      <c r="G1" s="5" t="s">
-        <v>24</v>
       </c>
       <c r="H1" s="5" t="s">
         <v>11</v>
@@ -834,22 +819,22 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D2" t="s">
         <v>2</v>
       </c>
       <c r="E2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F2" t="s">
         <v>12</v>
       </c>
       <c r="G2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
@@ -860,19 +845,42 @@
         <v>13</v>
       </c>
       <c r="C3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D3" t="s">
         <v>2</v>
       </c>
       <c r="E3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F3" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="G3" t="s">
-        <v>35</v>
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E4" t="s">
+        <v>39</v>
+      </c>
+      <c r="F4" t="s">
+        <v>16</v>
+      </c>
+      <c r="G4" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -898,7 +906,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -906,7 +914,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -914,10 +922,10 @@
         <v>2</v>
       </c>
       <c r="B4" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C4" t="s">
         <v>27</v>
-      </c>
-      <c r="C4" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
@@ -925,32 +933,32 @@
         <v>2</v>
       </c>
       <c r="B5" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5" t="s">
         <v>29</v>
-      </c>
-      <c r="C5" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B6" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="B6" s="5" t="s">
-        <v>32</v>
-      </c>
       <c r="C6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B7" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="B7" s="5" t="s">
-        <v>34</v>
-      </c>
       <c r="C7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed issue on dropping duplicates when adding units.
</commit_message>
<xml_diff>
--- a/conceptual test/master.xlsx
+++ b/conceptual test/master.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lorenzorinaldi/Documents/GitHub/SESAM/FIONA/conceptual test/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F3F9212-2F12-794A-9864-26D72553B909}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{516FAA53-081F-E149-B94B-B41A7C4932A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-9240" yWindow="-28300" windowWidth="51200" windowHeight="28300" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-9240" yWindow="-28300" windowWidth="51200" windowHeight="26880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Master" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="44">
   <si>
     <t>unit</t>
   </si>
@@ -153,6 +153,9 @@
   </si>
   <si>
     <t>Gsteel</t>
+  </si>
+  <si>
+    <t>Gsteel RoW</t>
   </si>
 </sst>
 </file>
@@ -564,10 +567,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:L2"/>
+  <dimension ref="A1:L3"/>
   <sheetViews>
-    <sheetView zoomScale="219" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" zoomScale="219" workbookViewId="0">
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -626,7 +629,7 @@
     </row>
     <row r="2" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B2" t="s">
         <v>40</v>
@@ -648,6 +651,29 @@
       </c>
       <c r="J2" t="s">
         <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D3" t="s">
+        <v>43</v>
+      </c>
+      <c r="E3" s="5">
+        <v>1</v>
+      </c>
+      <c r="F3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G3" s="9">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -662,7 +688,9 @@
   </sheetPr>
   <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -696,8 +724,8 @@
   </sheetPr>
   <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="240" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView zoomScale="240" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
changed filled_slices filling procedure from 'update' to '+='
</commit_message>
<xml_diff>
--- a/conceptual test/master.xlsx
+++ b/conceptual test/master.xlsx
@@ -8,23 +8,24 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lorenzorinaldi/Documents/GitHub/SESAM/FIONA/conceptual test/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BA223AC-177F-6A4D-9B0E-7AD016342B68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E48DA21-7255-2145-8E4E-4A4C41A3F662}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-9240" yWindow="-28300" windowWidth="51200" windowHeight="26880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17460" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Master" sheetId="1" r:id="rId1"/>
     <sheet name="Regions Map" sheetId="2" r:id="rId2"/>
-    <sheet name="Gsteel" sheetId="3" r:id="rId3"/>
-    <sheet name="Gsteel RoW" sheetId="5" r:id="rId4"/>
-    <sheet name="DB units" sheetId="4" r:id="rId5"/>
+    <sheet name="Gsteel" sheetId="5" r:id="rId3"/>
+    <sheet name="Test" sheetId="6" r:id="rId4"/>
+    <sheet name="Test2" sheetId="7" r:id="rId5"/>
+    <sheet name="DB units" sheetId="4" r:id="rId6"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="48">
   <si>
     <t>unit</t>
   </si>
@@ -155,7 +156,19 @@
     <t>Gsteel</t>
   </si>
   <si>
-    <t>Gsteel RoW</t>
+    <t>Test</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>Test1</t>
+  </si>
+  <si>
+    <t>Test2</t>
+  </si>
+  <si>
+    <t>test2</t>
   </si>
 </sst>
 </file>
@@ -568,10 +581,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:L3"/>
+  <dimension ref="A1:L4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="219" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+    <sheetView zoomScale="219" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -585,7 +598,7 @@
     <col min="7" max="7" width="11.33203125" style="9" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10.6640625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="11" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="9.1640625" bestFit="1" customWidth="1"/>
   </cols>
@@ -628,58 +641,78 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B2" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="C2" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="D2" t="s">
-        <v>42</v>
-      </c>
-      <c r="E2" s="5">
+        <v>43</v>
+      </c>
+      <c r="E2" s="9">
         <v>1</v>
       </c>
       <c r="F2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G2" s="5">
-        <v>1</v>
-      </c>
-      <c r="J2" t="s">
-        <v>5</v>
-      </c>
-      <c r="K2" t="b">
+        <v>44</v>
+      </c>
+      <c r="G2" s="9">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D3" t="s">
+        <v>46</v>
+      </c>
+      <c r="E3" s="9">
+        <v>1</v>
+      </c>
+      <c r="F3" t="s">
+        <v>47</v>
+      </c>
+      <c r="G3" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" t="s">
         <v>40</v>
       </c>
-      <c r="C3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" t="s">
-        <v>43</v>
-      </c>
-      <c r="E3" s="5">
-        <v>1</v>
-      </c>
-      <c r="F3" t="s">
+      <c r="C4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D4" t="s">
+        <v>42</v>
+      </c>
+      <c r="E4" s="5">
+        <v>1</v>
+      </c>
+      <c r="F4" t="s">
         <v>9</v>
       </c>
-      <c r="G3" s="9">
-        <v>1</v>
-      </c>
-      <c r="H3" s="10"/>
+      <c r="G4" s="9">
+        <v>1</v>
+      </c>
+      <c r="H4" s="10"/>
+      <c r="J4" t="s">
+        <v>5</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -723,14 +756,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FE6ACEF-2ADB-464D-8B15-AE40FEABD1BA}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView zoomScale="240" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -815,7 +848,7 @@
     </row>
     <row r="4" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="5">
-        <v>305</v>
+        <v>300</v>
       </c>
       <c r="B4" t="s">
         <v>12</v>
@@ -882,14 +915,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FE6ACEF-2ADB-464D-8B15-AE40FEABD1BA}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{939237FD-1F13-824E-B72F-F50316B1F0F8}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:H8"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView zoomScale="240" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3:E4"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -928,7 +961,7 @@
     </row>
     <row r="2" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4">
-        <v>0.52</v>
+        <v>1</v>
       </c>
       <c r="B2" t="s">
         <v>9</v>
@@ -951,7 +984,7 @@
     </row>
     <row r="3" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="4">
-        <v>9.7684465828781195E-2</v>
+        <v>1</v>
       </c>
       <c r="B3" t="s">
         <v>9</v>
@@ -966,7 +999,7 @@
         <v>41</v>
       </c>
       <c r="F3" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="G3" t="s">
         <v>26</v>
@@ -974,110 +1007,24 @@
     </row>
     <row r="4" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="4">
-        <v>0.05</v>
+        <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C4" t="s">
-        <v>27</v>
+        <v>6</v>
       </c>
       <c r="D4" t="s">
         <v>7</v>
       </c>
       <c r="E4" t="s">
-        <v>41</v>
+        <v>6</v>
       </c>
       <c r="F4" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="G4" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="5">
-        <v>300</v>
-      </c>
-      <c r="B5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D5" t="s">
-        <v>7</v>
-      </c>
-      <c r="E5" t="s">
-        <v>6</v>
-      </c>
-      <c r="F5" t="s">
-        <v>28</v>
-      </c>
-      <c r="G5" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="5">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D6" t="s">
-        <v>7</v>
-      </c>
-      <c r="E6" t="s">
-        <v>6</v>
-      </c>
-      <c r="F6" t="s">
-        <v>29</v>
-      </c>
-      <c r="G6" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="4">
-        <v>0.5</v>
-      </c>
-      <c r="B7" t="s">
-        <v>10</v>
-      </c>
-      <c r="C7" t="s">
-        <v>30</v>
-      </c>
-      <c r="D7" t="s">
-        <v>13</v>
-      </c>
-      <c r="E7" t="s">
-        <v>14</v>
-      </c>
-      <c r="G7" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="4">
-        <v>0.3</v>
-      </c>
-      <c r="B8" t="s">
-        <v>9</v>
-      </c>
-      <c r="C8" t="s">
-        <v>16</v>
-      </c>
-      <c r="D8" t="s">
-        <v>15</v>
-      </c>
-      <c r="E8" t="s">
-        <v>16</v>
-      </c>
-      <c r="G8" t="s">
         <v>26</v>
       </c>
     </row>
@@ -1087,6 +1034,125 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{217C4354-B707-1244-869E-C2C0E3D5B477}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:H4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="240" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="12.5" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17" bestFit="1" customWidth="1"/>
+    <col min="5" max="8" width="12.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="4">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="4">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" t="s">
+        <v>41</v>
+      </c>
+      <c r="F3" t="s">
+        <v>25</v>
+      </c>
+      <c r="G3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="4">
+        <v>1</v>
+      </c>
+      <c r="B4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F4" t="s">
+        <v>25</v>
+      </c>
+      <c r="G4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>

</xml_diff>